<commit_message>
change names in xlsx files
</commit_message>
<xml_diff>
--- a/templates/community/MibiNet/MibiNet_bioreactor_cultivation_conditions.xlsx
+++ b/templates/community/MibiNet/MibiNet_bioreactor_cultivation_conditions.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24332"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3DBE585-57EF-4D2F-8EBA-A7E79301B593}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BE4EA78-6178-47D8-B7C3-D6C88B98F0BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25215" yWindow="1170" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-24345" yWindow="2040" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="isa_template" sheetId="1" r:id="rId1"/>
@@ -375,7 +375,7 @@
     <t>http://purl.obolibrary.org/obo/UO_0000032</t>
   </si>
   <si>
-    <t>MibiNet_bioreactor_cultivation_conditions</t>
+    <t>MibiNet bioreactor cultivation conditions</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
delete space in Mibinet community name
</commit_message>
<xml_diff>
--- a/templates/community/MibiNet/MibiNet_bioreactor_cultivation_conditions.xlsx
+++ b/templates/community/MibiNet/MibiNet_bioreactor_cultivation_conditions.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27531"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BE4EA78-6178-47D8-B7C3-D6C88B98F0BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED131E6C-D390-408B-9E28-B69D11E581E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-24345" yWindow="2040" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="isa_template" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="119">
   <si>
     <t>TEMPLATE</t>
   </si>
@@ -43,9 +43,6 @@
   </si>
   <si>
     <t>Organisation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MibiNet </t>
   </si>
   <si>
     <t>Table</t>
@@ -856,7 +853,7 @@
   <dimension ref="A1:D28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -879,7 +876,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -903,156 +900,156 @@
         <v>8</v>
       </c>
       <c r="B6" t="s">
-        <v>9</v>
+        <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" t="s">
         <v>10</v>
-      </c>
-      <c r="B7" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" t="s">
         <v>17</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" t="s">
         <v>18</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
         <v>19</v>
-      </c>
-      <c r="D13" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" t="s">
         <v>21</v>
       </c>
-      <c r="B14" t="s">
+      <c r="C14" t="s">
         <v>22</v>
-      </c>
-      <c r="C14" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
+        <v>23</v>
+      </c>
+      <c r="B15" t="s">
         <v>24</v>
       </c>
-      <c r="B15" t="s">
+      <c r="C15" t="s">
         <v>25</v>
-      </c>
-      <c r="C15" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
+        <v>27</v>
+      </c>
+      <c r="B17" t="s">
         <v>28</v>
-      </c>
-      <c r="B17" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
+        <v>29</v>
+      </c>
+      <c r="B18" t="s">
         <v>30</v>
-      </c>
-      <c r="B18" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
+        <v>32</v>
+      </c>
+      <c r="B20" t="s">
         <v>33</v>
-      </c>
-      <c r="B20" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
+        <v>37</v>
+      </c>
+      <c r="B24" t="s">
         <v>38</v>
-      </c>
-      <c r="B24" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
+        <v>42</v>
+      </c>
+      <c r="B28" t="s">
         <v>43</v>
-      </c>
-      <c r="B28" t="s">
-        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -1071,354 +1068,354 @@
   <sheetData>
     <row r="1" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B1" t="s">
         <v>45</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>46</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>47</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>48</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>49</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>50</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>51</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>52</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>53</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>54</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>55</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>56</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>57</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>58</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>59</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>60</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>61</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>62</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>63</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>64</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>65</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>66</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>67</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>68</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>69</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
         <v>70</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AB1" t="s">
         <v>71</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AC1" t="s">
         <v>72</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AD1" t="s">
         <v>73</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AE1" t="s">
         <v>74</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AF1" t="s">
         <v>75</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AG1" t="s">
         <v>76</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AH1" t="s">
         <v>77</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AI1" t="s">
         <v>78</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AJ1" t="s">
         <v>79</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="AK1" t="s">
         <v>80</v>
       </c>
-      <c r="AK1" t="s">
+      <c r="AL1" t="s">
         <v>81</v>
       </c>
-      <c r="AL1" t="s">
+      <c r="AM1" t="s">
         <v>82</v>
       </c>
-      <c r="AM1" t="s">
+      <c r="AN1" t="s">
         <v>83</v>
       </c>
-      <c r="AN1" t="s">
+      <c r="AO1" t="s">
         <v>84</v>
       </c>
-      <c r="AO1" t="s">
+      <c r="AP1" t="s">
         <v>85</v>
       </c>
-      <c r="AP1" t="s">
+      <c r="AQ1" t="s">
         <v>86</v>
       </c>
-      <c r="AQ1" t="s">
+      <c r="AR1" t="s">
         <v>87</v>
       </c>
-      <c r="AR1" t="s">
+      <c r="AS1" t="s">
         <v>88</v>
       </c>
-      <c r="AS1" t="s">
+      <c r="AT1" t="s">
         <v>89</v>
       </c>
-      <c r="AT1" t="s">
+      <c r="AU1" t="s">
         <v>90</v>
       </c>
-      <c r="AU1" t="s">
+      <c r="AV1" t="s">
         <v>91</v>
       </c>
-      <c r="AV1" t="s">
+      <c r="AW1" t="s">
         <v>92</v>
       </c>
-      <c r="AW1" t="s">
+      <c r="AX1" t="s">
         <v>93</v>
       </c>
-      <c r="AX1" t="s">
+      <c r="AY1" t="s">
         <v>94</v>
       </c>
-      <c r="AY1" t="s">
+      <c r="AZ1" t="s">
         <v>95</v>
       </c>
-      <c r="AZ1" t="s">
+      <c r="BA1" t="s">
         <v>96</v>
       </c>
-      <c r="BA1" t="s">
+      <c r="BB1" t="s">
         <v>97</v>
       </c>
-      <c r="BB1" t="s">
+      <c r="BC1" t="s">
         <v>98</v>
       </c>
-      <c r="BC1" t="s">
+      <c r="BD1" t="s">
         <v>99</v>
       </c>
-      <c r="BD1" t="s">
+      <c r="BE1" t="s">
         <v>100</v>
       </c>
-      <c r="BE1" t="s">
+      <c r="BF1" t="s">
         <v>101</v>
-      </c>
-      <c r="BF1" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="2" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>102</v>
+      </c>
+      <c r="B2" t="s">
+        <v>102</v>
+      </c>
+      <c r="C2" t="s">
+        <v>102</v>
+      </c>
+      <c r="D2" t="s">
+        <v>102</v>
+      </c>
+      <c r="E2" t="s">
+        <v>102</v>
+      </c>
+      <c r="F2" t="s">
+        <v>102</v>
+      </c>
+      <c r="G2" t="s">
+        <v>102</v>
+      </c>
+      <c r="H2" t="s">
+        <v>102</v>
+      </c>
+      <c r="I2" t="s">
+        <v>102</v>
+      </c>
+      <c r="J2" t="s">
+        <v>102</v>
+      </c>
+      <c r="K2" t="s">
+        <v>102</v>
+      </c>
+      <c r="L2" t="s">
         <v>103</v>
       </c>
-      <c r="B2" t="s">
-        <v>103</v>
-      </c>
-      <c r="C2" t="s">
-        <v>103</v>
-      </c>
-      <c r="D2" t="s">
-        <v>103</v>
-      </c>
-      <c r="E2" t="s">
-        <v>103</v>
-      </c>
-      <c r="F2" t="s">
-        <v>103</v>
-      </c>
-      <c r="G2" t="s">
-        <v>103</v>
-      </c>
-      <c r="H2" t="s">
-        <v>103</v>
-      </c>
-      <c r="I2" t="s">
-        <v>103</v>
-      </c>
-      <c r="J2" t="s">
-        <v>103</v>
-      </c>
-      <c r="K2" t="s">
-        <v>103</v>
-      </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>104</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>105</v>
       </c>
-      <c r="N2" t="s">
+      <c r="O2" t="s">
+        <v>102</v>
+      </c>
+      <c r="P2" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>102</v>
+      </c>
+      <c r="R2" t="s">
+        <v>102</v>
+      </c>
+      <c r="S2" t="s">
+        <v>102</v>
+      </c>
+      <c r="T2" t="s">
+        <v>102</v>
+      </c>
+      <c r="U2" t="s">
+        <v>102</v>
+      </c>
+      <c r="V2" t="s">
+        <v>102</v>
+      </c>
+      <c r="W2" t="s">
+        <v>102</v>
+      </c>
+      <c r="X2" t="s">
+        <v>102</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>102</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>102</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>102</v>
+      </c>
+      <c r="AB2" t="s">
         <v>106</v>
       </c>
-      <c r="O2" t="s">
-        <v>103</v>
-      </c>
-      <c r="P2" t="s">
-        <v>103</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>103</v>
-      </c>
-      <c r="R2" t="s">
-        <v>103</v>
-      </c>
-      <c r="S2" t="s">
-        <v>103</v>
-      </c>
-      <c r="T2" t="s">
-        <v>103</v>
-      </c>
-      <c r="U2" t="s">
-        <v>103</v>
-      </c>
-      <c r="V2" t="s">
-        <v>103</v>
-      </c>
-      <c r="W2" t="s">
-        <v>103</v>
-      </c>
-      <c r="X2" t="s">
-        <v>103</v>
-      </c>
-      <c r="Y2" t="s">
-        <v>103</v>
-      </c>
-      <c r="Z2" t="s">
-        <v>103</v>
-      </c>
-      <c r="AA2" t="s">
-        <v>103</v>
-      </c>
-      <c r="AB2" t="s">
+      <c r="AC2" t="s">
         <v>107</v>
       </c>
-      <c r="AC2" t="s">
+      <c r="AD2" t="s">
         <v>108</v>
       </c>
-      <c r="AD2" t="s">
+      <c r="AE2" t="s">
+        <v>102</v>
+      </c>
+      <c r="AF2" t="s">
         <v>109</v>
       </c>
-      <c r="AE2" t="s">
-        <v>103</v>
-      </c>
-      <c r="AF2" t="s">
+      <c r="AG2" t="s">
+        <v>102</v>
+      </c>
+      <c r="AH2" t="s">
+        <v>102</v>
+      </c>
+      <c r="AI2" t="s">
+        <v>102</v>
+      </c>
+      <c r="AJ2" t="s">
         <v>110</v>
       </c>
-      <c r="AG2" t="s">
-        <v>103</v>
-      </c>
-      <c r="AH2" t="s">
-        <v>103</v>
-      </c>
-      <c r="AI2" t="s">
-        <v>103</v>
-      </c>
-      <c r="AJ2" t="s">
+      <c r="AK2" t="s">
+        <v>104</v>
+      </c>
+      <c r="AL2" t="s">
         <v>111</v>
       </c>
-      <c r="AK2" t="s">
-        <v>105</v>
-      </c>
-      <c r="AL2" t="s">
+      <c r="AM2" t="s">
+        <v>102</v>
+      </c>
+      <c r="AN2" t="s">
+        <v>110</v>
+      </c>
+      <c r="AO2" t="s">
+        <v>104</v>
+      </c>
+      <c r="AP2" t="s">
+        <v>111</v>
+      </c>
+      <c r="AQ2" t="s">
+        <v>102</v>
+      </c>
+      <c r="AR2" t="s">
+        <v>102</v>
+      </c>
+      <c r="AS2" t="s">
+        <v>102</v>
+      </c>
+      <c r="AT2" t="s">
+        <v>102</v>
+      </c>
+      <c r="AU2" t="s">
         <v>112</v>
       </c>
-      <c r="AM2" t="s">
-        <v>103</v>
-      </c>
-      <c r="AN2" t="s">
-        <v>111</v>
-      </c>
-      <c r="AO2" t="s">
-        <v>105</v>
-      </c>
-      <c r="AP2" t="s">
-        <v>112</v>
-      </c>
-      <c r="AQ2" t="s">
-        <v>103</v>
-      </c>
-      <c r="AR2" t="s">
-        <v>103</v>
-      </c>
-      <c r="AS2" t="s">
-        <v>103</v>
-      </c>
-      <c r="AT2" t="s">
-        <v>103</v>
-      </c>
-      <c r="AU2" t="s">
+      <c r="AV2" t="s">
+        <v>107</v>
+      </c>
+      <c r="AW2" t="s">
         <v>113</v>
       </c>
-      <c r="AV2" t="s">
-        <v>108</v>
-      </c>
-      <c r="AW2" t="s">
+      <c r="AX2" t="s">
+        <v>102</v>
+      </c>
+      <c r="AY2" t="s">
         <v>114</v>
       </c>
-      <c r="AX2" t="s">
-        <v>103</v>
-      </c>
-      <c r="AY2" t="s">
+      <c r="AZ2" t="s">
+        <v>104</v>
+      </c>
+      <c r="BA2" t="s">
         <v>115</v>
       </c>
-      <c r="AZ2" t="s">
-        <v>105</v>
-      </c>
-      <c r="BA2" t="s">
+      <c r="BB2" t="s">
+        <v>102</v>
+      </c>
+      <c r="BC2" t="s">
         <v>116</v>
       </c>
-      <c r="BB2" t="s">
-        <v>103</v>
-      </c>
-      <c r="BC2" t="s">
+      <c r="BD2" t="s">
+        <v>104</v>
+      </c>
+      <c r="BE2" t="s">
         <v>117</v>
       </c>
-      <c r="BD2" t="s">
-        <v>105</v>
-      </c>
-      <c r="BE2" t="s">
-        <v>118</v>
-      </c>
       <c r="BF2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add example data to MibiNet bioreactor template
</commit_message>
<xml_diff>
--- a/templates/community/MibiNet/MibiNet_bioreactor_cultivation_conditions.xlsx
+++ b/templates/community/MibiNet/MibiNet_bioreactor_cultivation_conditions.xlsx
@@ -1,22 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27531"/>
-  <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED131E6C-D390-408B-9E28-B69D11E581E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
-  <bookViews>
-    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
-  </bookViews>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
   <sheets>
-    <sheet name="isa_template" sheetId="1" r:id="rId1"/>
-    <sheet name="New Table" sheetId="2" r:id="rId2"/>
+    <sheet sheetId="1" name="isa_template" state="visible" r:id="rId4"/>
+    <sheet sheetId="2" name="Bioreactor cultivation conditio" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="137">
   <si>
     <t>TEMPLATE</t>
   </si>
@@ -30,10 +26,13 @@
     <t>Name</t>
   </si>
   <si>
+    <t>MibiNet bioreactor cultivation conditions</t>
+  </si>
+  <si>
     <t>Version</t>
   </si>
   <si>
-    <t>1.0.0</t>
+    <t>1.0.1</t>
   </si>
   <si>
     <t>Description</t>
@@ -45,10 +44,13 @@
     <t>Organisation</t>
   </si>
   <si>
+    <t>MibiNet</t>
+  </si>
+  <si>
     <t>Table</t>
   </si>
   <si>
-    <t>New Table</t>
+    <t>Bioreactor cultivation condition</t>
   </si>
   <si>
     <t>ERS</t>
@@ -132,9 +134,6 @@
     <t>Author Affiliation</t>
   </si>
   <si>
-    <t>MibiNet</t>
-  </si>
-  <si>
     <t>Author Roles</t>
   </si>
   <si>
@@ -321,19 +320,52 @@
     <t xml:space="preserve">Term Accession Number ()    </t>
   </si>
   <si>
-    <t>Output [Raw Data File]</t>
+    <t>Output [Data]</t>
   </si>
   <si>
     <t/>
   </si>
   <si>
+    <t>A1</t>
+  </si>
+  <si>
+    <t>Corynebacterium glutamicum</t>
+  </si>
+  <si>
+    <t>NCBITaxon</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCBITaxon_1718</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CGXII medium 2% Glucose </t>
+  </si>
+  <si>
+    <t>0,75</t>
+  </si>
+  <si>
     <t>milliliter</t>
   </si>
   <si>
     <t>UO</t>
   </si>
   <si>
-    <t>http://purl.obolibrary.org/obo/UO_0000098</t>
+    <t>https://bioregistry.io/UO:0000098</t>
+  </si>
+  <si>
+    <t>0,5</t>
+  </si>
+  <si>
+    <t>BL127_CX-269C62</t>
+  </si>
+  <si>
+    <t>MTP-48-FlowerPlate</t>
+  </si>
+  <si>
+    <t>eYFP (508, 532 nm)</t>
+  </si>
+  <si>
+    <t>30</t>
   </si>
   <si>
     <t>Degree Celsius</t>
@@ -342,50 +374,68 @@
     <t>NCIT</t>
   </si>
   <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C42559</t>
+    <t>https://bioregistry.io/NCIT:C42559</t>
+  </si>
+  <si>
+    <t>85</t>
   </si>
   <si>
     <t>rH</t>
   </si>
   <si>
+    <t>20,95</t>
+  </si>
+  <si>
     <t>percent</t>
   </si>
   <si>
-    <t>http://purl.obolibrary.org/obo/UO_0000187</t>
+    <t>https://bioregistry.io/UO:0000187</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>7,0</t>
+  </si>
+  <si>
+    <t>1200</t>
   </si>
   <si>
     <t>Revolution per Minute</t>
   </si>
   <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C70469</t>
+    <t>https://bioregistry.io/NCIT:C70469</t>
+  </si>
+  <si>
+    <t>15</t>
   </si>
   <si>
     <t>minute</t>
   </si>
   <si>
-    <t>http://purl.obolibrary.org/obo/UO_0000031</t>
+    <t>https://bioregistry.io/UO:0000031</t>
+  </si>
+  <si>
+    <t>1193</t>
   </si>
   <si>
     <t>hour</t>
   </si>
   <si>
-    <t>http://purl.obolibrary.org/obo/UO_0000032</t>
-  </si>
-  <si>
-    <t>MibiNet bioreactor cultivation conditions</t>
+    <t>https://bioregistry.io/UO:0000032</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+      <sz val="11"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
@@ -412,7 +462,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -428,8 +478,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="annotationTable" displayName="annotationTable" ref="A1:BF2">
-  <autoFilter ref="A1:BF2" xr:uid="{00000000-0009-0000-0100-000001000000}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" name="annotationTable" displayName="annotationTable" ref="A1:BF2" totalsRowShown="1" headerRowCount="1">
+  <autoFilter ref="A1:BF2">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -490,64 +540,64 @@
     <filterColumn colId="57" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="58">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Input [Sample Name]" totalsRowLabel="Total"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Parameter [Well]"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Term Source REF (NFDI4PSO:1000101)"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Term Accession Number (NFDI4PSO:1000101)"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Characteristic [Organism]"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Term Source REF (MIAPPE:0041)"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Term Accession Number (MIAPPE:0041)"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Parameter [Growth Medium]"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Term Source REF (NCIT:C85504)"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Term Accession Number (NCIT:C85504)"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Parameter [culture medium volume]"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Unit"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="Term Source REF (DPBO:1000155)"/>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="Term Accession Number (DPBO:1000155)"/>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="Parameter [start OD600]"/>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="Term Source REF (DPBO:0000101)"/>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="Term Accession Number (DPBO:0000101)"/>
-    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="Component [cultivation device]"/>
-    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" name="Term Source REF ()"/>
-    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0000-000014000000}" name="Term Accession Number ()"/>
-    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0000-000015000000}" name="Parameter [sample plate type]"/>
-    <tableColumn id="22" xr3:uid="{00000000-0010-0000-0000-000016000000}" name="Term Source REF (MS:1001938)"/>
-    <tableColumn id="23" xr3:uid="{00000000-0010-0000-0000-000017000000}" name="Term Accession Number (MS:1001938)"/>
-    <tableColumn id="24" xr3:uid="{00000000-0010-0000-0000-000018000000}" name="Parameter [filterset]"/>
-    <tableColumn id="25" xr3:uid="{00000000-0010-0000-0000-000019000000}" name="Term Source REF () "/>
-    <tableColumn id="26" xr3:uid="{00000000-0010-0000-0000-00001A000000}" name="Term Accession Number () "/>
-    <tableColumn id="27" xr3:uid="{00000000-0010-0000-0000-00001B000000}" name="Parameter [temperature]"/>
-    <tableColumn id="28" xr3:uid="{00000000-0010-0000-0000-00001C000000}" name="Unit "/>
-    <tableColumn id="29" xr3:uid="{00000000-0010-0000-0000-00001D000000}" name="Term Source REF (EFO:0001702)"/>
-    <tableColumn id="30" xr3:uid="{00000000-0010-0000-0000-00001E000000}" name="Term Accession Number (EFO:0001702)"/>
-    <tableColumn id="31" xr3:uid="{00000000-0010-0000-0000-00001F000000}" name="Parameter [humidity]"/>
-    <tableColumn id="32" xr3:uid="{00000000-0010-0000-0000-000020000000}" name="Unit  "/>
-    <tableColumn id="33" xr3:uid="{00000000-0010-0000-0000-000021000000}" name="Term Source REF (PATO:0015009)"/>
-    <tableColumn id="34" xr3:uid="{00000000-0010-0000-0000-000022000000}" name="Term Accession Number (PATO:0015009)"/>
-    <tableColumn id="35" xr3:uid="{00000000-0010-0000-0000-000023000000}" name="Parameter [Oxygen]"/>
-    <tableColumn id="36" xr3:uid="{00000000-0010-0000-0000-000024000000}" name="Unit   "/>
-    <tableColumn id="37" xr3:uid="{00000000-0010-0000-0000-000025000000}" name="Term Source REF (NCIT:C722)"/>
-    <tableColumn id="38" xr3:uid="{00000000-0010-0000-0000-000026000000}" name="Term Accession Number (NCIT:C722)"/>
-    <tableColumn id="39" xr3:uid="{00000000-0010-0000-0000-000027000000}" name="Parameter [Carbon Dioxide]"/>
-    <tableColumn id="40" xr3:uid="{00000000-0010-0000-0000-000028000000}" name="Unit    "/>
-    <tableColumn id="41" xr3:uid="{00000000-0010-0000-0000-000029000000}" name="Term Source REF (NCIT:C65288)"/>
-    <tableColumn id="42" xr3:uid="{00000000-0010-0000-0000-00002A000000}" name="Term Accession Number (NCIT:C65288)"/>
-    <tableColumn id="43" xr3:uid="{00000000-0010-0000-0000-00002B000000}" name="Parameter [pH]"/>
-    <tableColumn id="44" xr3:uid="{00000000-0010-0000-0000-00002C000000}" name="Term Source REF (UO:0000196)"/>
-    <tableColumn id="45" xr3:uid="{00000000-0010-0000-0000-00002D000000}" name="Term Accession Number (UO:0000196)"/>
-    <tableColumn id="46" xr3:uid="{00000000-0010-0000-0000-00002E000000}" name="Parameter [shaker frequency]"/>
-    <tableColumn id="47" xr3:uid="{00000000-0010-0000-0000-00002F000000}" name="Unit     "/>
-    <tableColumn id="48" xr3:uid="{00000000-0010-0000-0000-000030000000}" name="Term Source REF ()  "/>
-    <tableColumn id="49" xr3:uid="{00000000-0010-0000-0000-000031000000}" name="Term Accession Number ()  "/>
-    <tableColumn id="50" xr3:uid="{00000000-0010-0000-0000-000032000000}" name="Parameter [cycle time]"/>
-    <tableColumn id="51" xr3:uid="{00000000-0010-0000-0000-000033000000}" name="Unit      "/>
-    <tableColumn id="52" xr3:uid="{00000000-0010-0000-0000-000034000000}" name="Term Source REF ()   "/>
-    <tableColumn id="53" xr3:uid="{00000000-0010-0000-0000-000035000000}" name="Term Accession Number ()   "/>
-    <tableColumn id="54" xr3:uid="{00000000-0010-0000-0000-000036000000}" name="Parameter [experiment time]"/>
-    <tableColumn id="55" xr3:uid="{00000000-0010-0000-0000-000037000000}" name="Unit       "/>
-    <tableColumn id="56" xr3:uid="{00000000-0010-0000-0000-000038000000}" name="Term Source REF ()    "/>
-    <tableColumn id="57" xr3:uid="{00000000-0010-0000-0000-000039000000}" name="Term Accession Number ()    "/>
-    <tableColumn id="58" xr3:uid="{00000000-0010-0000-0000-00003A000000}" name="Output [Raw Data File]"/>
+    <tableColumn id="1" name="Input [Sample Name]" totalsRowLabel="Total"/>
+    <tableColumn id="2" name="Parameter [Well]" totalsRowFunction="none"/>
+    <tableColumn id="3" name="Term Source REF (NFDI4PSO:1000101)" totalsRowFunction="none"/>
+    <tableColumn id="4" name="Term Accession Number (NFDI4PSO:1000101)" totalsRowFunction="none"/>
+    <tableColumn id="5" name="Characteristic [Organism]" totalsRowFunction="none"/>
+    <tableColumn id="6" name="Term Source REF (MIAPPE:0041)" totalsRowFunction="none"/>
+    <tableColumn id="7" name="Term Accession Number (MIAPPE:0041)" totalsRowFunction="none"/>
+    <tableColumn id="8" name="Parameter [Growth Medium]" totalsRowFunction="none"/>
+    <tableColumn id="9" name="Term Source REF (NCIT:C85504)" totalsRowFunction="none"/>
+    <tableColumn id="10" name="Term Accession Number (NCIT:C85504)" totalsRowFunction="none"/>
+    <tableColumn id="11" name="Parameter [culture medium volume]" totalsRowFunction="none"/>
+    <tableColumn id="12" name="Unit" totalsRowFunction="none"/>
+    <tableColumn id="13" name="Term Source REF (DPBO:1000155)" totalsRowFunction="none"/>
+    <tableColumn id="14" name="Term Accession Number (DPBO:1000155)" totalsRowFunction="none"/>
+    <tableColumn id="15" name="Parameter [start OD600]" totalsRowFunction="none"/>
+    <tableColumn id="16" name="Term Source REF (DPBO:0000101)" totalsRowFunction="none"/>
+    <tableColumn id="17" name="Term Accession Number (DPBO:0000101)" totalsRowFunction="none"/>
+    <tableColumn id="18" name="Component [cultivation device]" totalsRowFunction="none"/>
+    <tableColumn id="19" name="Term Source REF ()" totalsRowFunction="none"/>
+    <tableColumn id="20" name="Term Accession Number ()" totalsRowFunction="none"/>
+    <tableColumn id="21" name="Parameter [sample plate type]" totalsRowFunction="none"/>
+    <tableColumn id="22" name="Term Source REF (MS:1001938)" totalsRowFunction="none"/>
+    <tableColumn id="23" name="Term Accession Number (MS:1001938)" totalsRowFunction="none"/>
+    <tableColumn id="24" name="Parameter [filterset]" totalsRowFunction="none"/>
+    <tableColumn id="25" name="Term Source REF () " totalsRowFunction="none"/>
+    <tableColumn id="26" name="Term Accession Number () " totalsRowFunction="none"/>
+    <tableColumn id="27" name="Parameter [temperature]" totalsRowFunction="none"/>
+    <tableColumn id="28" name="Unit " totalsRowFunction="none"/>
+    <tableColumn id="29" name="Term Source REF (EFO:0001702)" totalsRowFunction="none"/>
+    <tableColumn id="30" name="Term Accession Number (EFO:0001702)" totalsRowFunction="none"/>
+    <tableColumn id="31" name="Parameter [humidity]" totalsRowFunction="none"/>
+    <tableColumn id="32" name="Unit  " totalsRowFunction="none"/>
+    <tableColumn id="33" name="Term Source REF (PATO:0015009)" totalsRowFunction="none"/>
+    <tableColumn id="34" name="Term Accession Number (PATO:0015009)" totalsRowFunction="none"/>
+    <tableColumn id="35" name="Parameter [Oxygen]" totalsRowFunction="none"/>
+    <tableColumn id="36" name="Unit   " totalsRowFunction="none"/>
+    <tableColumn id="37" name="Term Source REF (NCIT:C722)" totalsRowFunction="none"/>
+    <tableColumn id="38" name="Term Accession Number (NCIT:C722)" totalsRowFunction="none"/>
+    <tableColumn id="39" name="Parameter [Carbon Dioxide]" totalsRowFunction="none"/>
+    <tableColumn id="40" name="Unit    " totalsRowFunction="none"/>
+    <tableColumn id="41" name="Term Source REF (NCIT:C65288)" totalsRowFunction="none"/>
+    <tableColumn id="42" name="Term Accession Number (NCIT:C65288)" totalsRowFunction="none"/>
+    <tableColumn id="43" name="Parameter [pH]" totalsRowFunction="none"/>
+    <tableColumn id="44" name="Term Source REF (UO:0000196)" totalsRowFunction="none"/>
+    <tableColumn id="45" name="Term Accession Number (UO:0000196)" totalsRowFunction="none"/>
+    <tableColumn id="46" name="Parameter [shaker frequency]" totalsRowFunction="none"/>
+    <tableColumn id="47" name="Unit     " totalsRowFunction="none"/>
+    <tableColumn id="48" name="Term Source REF ()  " totalsRowFunction="none"/>
+    <tableColumn id="49" name="Term Accession Number ()  " totalsRowFunction="none"/>
+    <tableColumn id="50" name="Parameter [cycle time]" totalsRowFunction="none"/>
+    <tableColumn id="51" name="Unit      " totalsRowFunction="none"/>
+    <tableColumn id="52" name="Term Source REF ()   " totalsRowFunction="none"/>
+    <tableColumn id="53" name="Term Accession Number ()   " totalsRowFunction="none"/>
+    <tableColumn id="54" name="Parameter [experiment time]" totalsRowFunction="none"/>
+    <tableColumn id="55" name="Unit       " totalsRowFunction="none"/>
+    <tableColumn id="56" name="Term Source REF ()    " totalsRowFunction="none"/>
+    <tableColumn id="57" name="Term Accession Number ()    " totalsRowFunction="none"/>
+    <tableColumn id="58" name="Output [Data]" totalsRowFunction="none"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -849,21 +899,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D28"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -871,556 +916,553 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13" t="s">
+        <v>19</v>
+      </c>
+      <c r="C13" t="s">
+        <v>20</v>
+      </c>
+      <c r="D13" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>22</v>
+      </c>
+      <c r="B14" t="s">
+        <v>23</v>
+      </c>
+      <c r="C14" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>25</v>
+      </c>
+      <c r="B15" t="s">
+        <v>26</v>
+      </c>
+      <c r="C15" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>29</v>
+      </c>
+      <c r="B17" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>31</v>
+      </c>
+      <c r="B18" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>34</v>
+      </c>
+      <c r="B20" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" t="s">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>39</v>
+      </c>
+      <c r="B24" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>16</v>
-      </c>
-      <c r="B13" t="s">
-        <v>17</v>
-      </c>
-      <c r="C13" t="s">
-        <v>18</v>
-      </c>
-      <c r="D13" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>20</v>
-      </c>
-      <c r="B14" t="s">
-        <v>21</v>
-      </c>
-      <c r="C14" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>23</v>
-      </c>
-      <c r="B15" t="s">
-        <v>24</v>
-      </c>
-      <c r="C15" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>27</v>
-      </c>
-      <c r="B17" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>29</v>
-      </c>
-      <c r="B18" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>32</v>
-      </c>
-      <c r="B20" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
-        <v>37</v>
-      </c>
-      <c r="B24" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B28" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BF2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
-    <row r="1" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="F1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="G1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="H1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="I1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="J1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="K1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="L1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="M1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="N1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="O1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="P1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="Q1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="R1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="S1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="T1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="U1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="V1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="W1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="X1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="Y1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="Z1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="AA1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="AB1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="AC1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="AD1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="AE1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="AF1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="AG1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="AH1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="AI1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="AJ1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="AK1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="AL1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="AM1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="AN1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="AO1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="AP1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="AQ1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="AR1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="AS1" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="AT1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="AU1" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="AV1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="AW1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="AX1" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="AY1" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="AZ1" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="BA1" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="BB1" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="BC1" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="BD1" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="BE1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="BF1" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="2" spans="1:58" x14ac:dyDescent="0.3">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="2" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B2" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="C2" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D2" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="E2" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="F2" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="G2" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
       <c r="H2" t="s">
-        <v>102</v>
+        <v>108</v>
       </c>
       <c r="I2" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="J2" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="K2" t="s">
-        <v>102</v>
+        <v>109</v>
       </c>
       <c r="L2" t="s">
-        <v>103</v>
+        <v>110</v>
       </c>
       <c r="M2" t="s">
-        <v>104</v>
+        <v>111</v>
       </c>
       <c r="N2" t="s">
-        <v>105</v>
+        <v>112</v>
       </c>
       <c r="O2" t="s">
-        <v>102</v>
+        <v>113</v>
       </c>
       <c r="P2" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="Q2" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="R2" t="s">
-        <v>102</v>
+        <v>114</v>
       </c>
       <c r="S2" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="T2" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="U2" t="s">
-        <v>102</v>
+        <v>115</v>
       </c>
       <c r="V2" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="W2" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="X2" t="s">
-        <v>102</v>
+        <v>116</v>
       </c>
       <c r="Y2" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="Z2" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="AA2" t="s">
-        <v>102</v>
+        <v>117</v>
       </c>
       <c r="AB2" t="s">
-        <v>106</v>
+        <v>118</v>
       </c>
       <c r="AC2" t="s">
-        <v>107</v>
+        <v>119</v>
       </c>
       <c r="AD2" t="s">
-        <v>108</v>
+        <v>120</v>
       </c>
       <c r="AE2" t="s">
-        <v>102</v>
+        <v>121</v>
       </c>
       <c r="AF2" t="s">
-        <v>109</v>
+        <v>122</v>
       </c>
       <c r="AG2" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="AH2" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="AI2" t="s">
-        <v>102</v>
+        <v>123</v>
       </c>
       <c r="AJ2" t="s">
-        <v>110</v>
+        <v>124</v>
       </c>
       <c r="AK2" t="s">
-        <v>104</v>
+        <v>111</v>
       </c>
       <c r="AL2" t="s">
+        <v>125</v>
+      </c>
+      <c r="AM2" t="s">
+        <v>126</v>
+      </c>
+      <c r="AN2" t="s">
+        <v>124</v>
+      </c>
+      <c r="AO2" t="s">
         <v>111</v>
       </c>
-      <c r="AM2" t="s">
-        <v>102</v>
-      </c>
-      <c r="AN2" t="s">
-        <v>110</v>
-      </c>
-      <c r="AO2" t="s">
-        <v>104</v>
-      </c>
       <c r="AP2" t="s">
+        <v>125</v>
+      </c>
+      <c r="AQ2" t="s">
+        <v>127</v>
+      </c>
+      <c r="AR2" t="s">
+        <v>103</v>
+      </c>
+      <c r="AS2" t="s">
+        <v>103</v>
+      </c>
+      <c r="AT2" t="s">
+        <v>128</v>
+      </c>
+      <c r="AU2" t="s">
+        <v>129</v>
+      </c>
+      <c r="AV2" t="s">
+        <v>119</v>
+      </c>
+      <c r="AW2" t="s">
+        <v>130</v>
+      </c>
+      <c r="AX2" t="s">
+        <v>131</v>
+      </c>
+      <c r="AY2" t="s">
+        <v>132</v>
+      </c>
+      <c r="AZ2" t="s">
         <v>111</v>
       </c>
-      <c r="AQ2" t="s">
-        <v>102</v>
-      </c>
-      <c r="AR2" t="s">
-        <v>102</v>
-      </c>
-      <c r="AS2" t="s">
-        <v>102</v>
-      </c>
-      <c r="AT2" t="s">
-        <v>102</v>
-      </c>
-      <c r="AU2" t="s">
-        <v>112</v>
-      </c>
-      <c r="AV2" t="s">
-        <v>107</v>
-      </c>
-      <c r="AW2" t="s">
-        <v>113</v>
-      </c>
-      <c r="AX2" t="s">
-        <v>102</v>
-      </c>
-      <c r="AY2" t="s">
-        <v>114</v>
-      </c>
-      <c r="AZ2" t="s">
-        <v>104</v>
-      </c>
       <c r="BA2" t="s">
-        <v>115</v>
+        <v>133</v>
       </c>
       <c r="BB2" t="s">
-        <v>102</v>
+        <v>134</v>
       </c>
       <c r="BC2" t="s">
-        <v>116</v>
+        <v>135</v>
       </c>
       <c r="BD2" t="s">
-        <v>104</v>
+        <v>111</v>
       </c>
       <c r="BE2" t="s">
-        <v>117</v>
+        <v>136</v>
       </c>
       <c r="BF2" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
   </tableParts>

</xml_diff>